<commit_message>
编写微车V2.4.1详细用例to be continue by Trais
</commit_message>
<xml_diff>
--- a/Buding_Secondary_TestCases/Weiche/布丁微车V2.4.1测试用例.xlsx
+++ b/Buding_Secondary_TestCases/Weiche/布丁微车V2.4.1测试用例.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" tabRatio="631" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" tabRatio="631"/>
   </bookViews>
   <sheets>
     <sheet name="首页M" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="230">
   <si>
     <t>测试项</t>
   </si>
@@ -1164,6 +1164,70 @@
   </si>
   <si>
     <t>1. 弹出“行车记录仪介绍”对话框</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试设备未联网</t>
+  </si>
+  <si>
+    <t>网络环境测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试设备连接可用Wifi</t>
+  </si>
+  <si>
+    <t>测试设备连接2G</t>
+  </si>
+  <si>
+    <t>测试设备连接3G</t>
+  </si>
+  <si>
+    <t>测试设备连接无外网Wifi</t>
+  </si>
+  <si>
+    <t>1. 执行以上用例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 应用可正常使用
+2. 数据加载正常</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 应用可正常使用
+2. 数据无法完成更新，存在网络请求时，提示“网络存在问题”提示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>升级测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 使用新版本对原有已发布版本进行覆盖安装测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>系统兼容性测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备兼容性测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 使用不同系统版本的设备
+2. 执行以上用例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 应用可正常使用，应用页面显示正常
+2. 数据加载正常</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 使用不同硬件配置的设备
+2. 执行以上用例</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1302,7 +1366,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1342,18 +1406,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1390,11 +1442,245 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="76">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2381,10 +2667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2422,7 +2708,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="33">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="26" t="s">
         <v>99</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -2443,7 +2729,7 @@
       <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="115.5">
-      <c r="A3" s="14"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
@@ -2456,12 +2742,12 @@
       <c r="E3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="23" t="s">
         <v>123</v>
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="14.25" customHeight="1">
+    <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="6"/>
       <c r="C4" s="3"/>
@@ -2472,15 +2758,15 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="12"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="3"/>
+      <c r="A6" s="2"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -2488,26 +2774,16 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="G4:G5"/>
+  <mergeCells count="1">
     <mergeCell ref="A2:A3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="57" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2525,43 +2801,43 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="13.875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="23" customWidth="1"/>
-    <col min="3" max="4" width="16.375" style="20" customWidth="1"/>
-    <col min="5" max="5" width="33.125" style="20" customWidth="1"/>
-    <col min="6" max="6" width="61.875" style="20" customWidth="1"/>
-    <col min="7" max="7" width="8.125" style="20" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="20"/>
+    <col min="1" max="1" width="13.875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.875" style="19" customWidth="1"/>
+    <col min="3" max="4" width="16.375" style="16" customWidth="1"/>
+    <col min="5" max="5" width="33.125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="61.875" style="16" customWidth="1"/>
+    <col min="7" max="7" width="8.125" style="16" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="20" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2569,30 +2845,186 @@
       <c r="A2" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="G2" s="27"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="1:7" ht="49.5">
+      <c r="A3" s="28"/>
+      <c r="B3" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:7" ht="33">
+      <c r="A4" s="28"/>
+      <c r="B4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="E4" s="28"/>
+      <c r="F4" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="1:7" ht="33">
+      <c r="A5" s="28"/>
+      <c r="B5" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="E5" s="28"/>
+      <c r="F5" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="1:7" ht="33.75" customHeight="1">
+      <c r="A6" s="28"/>
+      <c r="B6" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="E6" s="28"/>
+      <c r="F6" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="G6" s="23"/>
+    </row>
+    <row r="7" spans="1:7" ht="33">
+      <c r="A7" s="28"/>
+      <c r="B7" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="E7" s="28"/>
+      <c r="F7" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="G7" s="23"/>
+    </row>
+    <row r="8" spans="1:7" ht="33">
+      <c r="A8" s="28"/>
+      <c r="B8" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="28"/>
+      <c r="D8" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="E8" s="28"/>
+      <c r="F8" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="G8" s="23"/>
+    </row>
+    <row r="9" spans="1:7" ht="49.5">
+      <c r="A9" s="28"/>
+      <c r="B9" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>223</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="G9" s="23"/>
+    </row>
+    <row r="10" spans="1:7" ht="49.5">
+      <c r="A10" s="28"/>
+      <c r="B10" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="G10" s="23"/>
+    </row>
+    <row r="11" spans="1:7" ht="49.5">
+      <c r="A11" s="28"/>
+      <c r="B11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="G11" s="23"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="E3:E8"/>
+    <mergeCell ref="A2:A11"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2605,6 +3037,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2626,7 +3059,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2664,7 +3097,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="49.5">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="28" t="s">
         <v>100</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -2685,7 +3118,7 @@
       <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:8" ht="66">
-      <c r="A3" s="15"/>
+      <c r="A3" s="28"/>
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
@@ -2704,7 +3137,7 @@
       <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:8" ht="49.5">
-      <c r="A4" s="15"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="9" t="s">
         <v>16</v>
       </c>
@@ -2723,7 +3156,7 @@
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:8" ht="66">
-      <c r="A5" s="15"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="9" t="s">
         <v>67</v>
       </c>
@@ -2766,10 +3199,10 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="H9" s="12"/>
+      <c r="H9" s="25"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="H10" s="12"/>
+      <c r="H10" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2778,18 +3211,18 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="55" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="3" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H10">
-    <cfRule type="cellIs" dxfId="53" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2825,209 +3258,209 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="20" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="132">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="23" t="s">
         <v>176</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="G2" s="27"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:7" ht="132">
-      <c r="A3" s="15"/>
-      <c r="B3" s="26" t="s">
+      <c r="A3" s="28"/>
+      <c r="B3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="27"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:7" ht="82.5">
-      <c r="A4" s="15"/>
-      <c r="B4" s="26" t="s">
+      <c r="A4" s="28"/>
+      <c r="B4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="G4" s="27"/>
-    </row>
-    <row r="5" spans="1:7" s="20" customFormat="1" ht="82.5">
-      <c r="A5" s="15"/>
-      <c r="B5" s="26" t="s">
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="1:7" s="16" customFormat="1" ht="82.5">
+      <c r="A5" s="28"/>
+      <c r="B5" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="G5" s="27"/>
-    </row>
-    <row r="6" spans="1:7" s="20" customFormat="1" ht="66">
-      <c r="A6" s="15"/>
-      <c r="B6" s="26" t="s">
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="1:7" s="16" customFormat="1" ht="66">
+      <c r="A6" s="28"/>
+      <c r="B6" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="G6" s="27"/>
-    </row>
-    <row r="7" spans="1:7" s="20" customFormat="1" ht="82.5" customHeight="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="26" t="s">
+      <c r="G6" s="23"/>
+    </row>
+    <row r="7" spans="1:7" s="16" customFormat="1" ht="82.5" customHeight="1">
+      <c r="A7" s="28"/>
+      <c r="B7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="G7" s="27"/>
-    </row>
-    <row r="8" spans="1:7" s="20" customFormat="1" ht="82.5" customHeight="1">
-      <c r="A8" s="15"/>
-      <c r="B8" s="26" t="s">
+      <c r="G7" s="23"/>
+    </row>
+    <row r="8" spans="1:7" s="16" customFormat="1" ht="82.5" customHeight="1">
+      <c r="A8" s="28"/>
+      <c r="B8" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="27"/>
-    </row>
-    <row r="9" spans="1:7" s="20" customFormat="1" ht="132" customHeight="1">
-      <c r="A9" s="15"/>
-      <c r="B9" s="26" t="s">
+      <c r="F8" s="28"/>
+      <c r="G8" s="23"/>
+    </row>
+    <row r="9" spans="1:7" s="16" customFormat="1" ht="132" customHeight="1">
+      <c r="A9" s="28"/>
+      <c r="B9" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="G9" s="27"/>
-    </row>
-    <row r="10" spans="1:7" s="20" customFormat="1" ht="99" customHeight="1">
-      <c r="A10" s="15"/>
-      <c r="B10" s="26" t="s">
+      <c r="G9" s="23"/>
+    </row>
+    <row r="10" spans="1:7" s="16" customFormat="1" ht="99" customHeight="1">
+      <c r="A10" s="28"/>
+      <c r="B10" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="27"/>
-    </row>
-    <row r="11" spans="1:7" s="20" customFormat="1" ht="99" customHeight="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="26" t="s">
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="23"/>
+    </row>
+    <row r="11" spans="1:7" s="16" customFormat="1" ht="99" customHeight="1">
+      <c r="A11" s="28"/>
+      <c r="B11" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="27"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3038,10 +3471,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3100,7 +3533,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="99">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="26" t="s">
         <v>102</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -3121,7 +3554,7 @@
       <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="49.5">
-      <c r="A3" s="16"/>
+      <c r="A3" s="29"/>
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
@@ -3140,7 +3573,7 @@
       <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" ht="49.5">
-      <c r="A4" s="16"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="9" t="s">
         <v>16</v>
       </c>
@@ -3153,13 +3586,13 @@
       <c r="E4" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="23" t="s">
         <v>120</v>
       </c>
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" ht="49.5">
-      <c r="A5" s="16"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
@@ -3172,13 +3605,13 @@
       <c r="E5" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="23" t="s">
         <v>117</v>
       </c>
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" ht="49.5">
-      <c r="A6" s="16"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="9" t="s">
         <v>15</v>
       </c>
@@ -3197,7 +3630,7 @@
       <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:7" ht="33">
-      <c r="A7" s="16"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="9" t="s">
         <v>17</v>
       </c>
@@ -3216,15 +3649,15 @@
       <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
     </row>
     <row r="9" spans="1:7" ht="132">
       <c r="A9" s="11" t="s">
@@ -3253,10 +3686,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="47" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="3" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3316,7 +3749,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="148.5">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="26" t="s">
         <v>103</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -3337,7 +3770,7 @@
       <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="132">
-      <c r="A3" s="16"/>
+      <c r="A3" s="29"/>
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
@@ -3356,7 +3789,7 @@
       <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" ht="148.5">
-      <c r="A4" s="16"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="9" t="s">
         <v>16</v>
       </c>
@@ -3375,7 +3808,7 @@
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" ht="148.5">
-      <c r="A5" s="16"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
@@ -3394,7 +3827,7 @@
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" ht="82.5">
-      <c r="A6" s="16"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="9" t="s">
         <v>15</v>
       </c>
@@ -3413,7 +3846,7 @@
       <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:7" ht="49.5">
-      <c r="A7" s="16"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="9" t="s">
         <v>17</v>
       </c>
@@ -3432,7 +3865,7 @@
       <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" ht="49.5">
-      <c r="A8" s="16"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="9" t="s">
         <v>55</v>
       </c>
@@ -3451,7 +3884,7 @@
       <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" ht="66">
-      <c r="A9" s="16"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="9" t="s">
         <v>56</v>
       </c>
@@ -3470,7 +3903,7 @@
       <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:7" ht="33">
-      <c r="A10" s="14"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="9" t="s">
         <v>57</v>
       </c>
@@ -3494,10 +3927,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="3" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3518,7 +3951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -3534,143 +3967,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="20" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="66">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="G2" s="27"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:8" ht="66">
-      <c r="A3" s="15"/>
-      <c r="B3" s="26" t="s">
+      <c r="A3" s="28"/>
+      <c r="B3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="G3" s="27"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:8" ht="66">
-      <c r="A4" s="15"/>
-      <c r="B4" s="26" t="s">
+      <c r="A4" s="28"/>
+      <c r="B4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="G4" s="27"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:8" ht="66">
-      <c r="A5" s="15"/>
-      <c r="B5" s="26" t="s">
+      <c r="A5" s="28"/>
+      <c r="B5" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="G5" s="27"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:8" ht="66">
-      <c r="A6" s="15"/>
-      <c r="B6" s="26" t="s">
+      <c r="A6" s="28"/>
+      <c r="B6" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="27"/>
-    </row>
-    <row r="7" spans="1:8" s="20" customFormat="1" ht="66">
-      <c r="A7" s="15"/>
-      <c r="B7" s="26" t="s">
+      <c r="G6" s="23"/>
+    </row>
+    <row r="7" spans="1:8" s="16" customFormat="1" ht="66">
+      <c r="A7" s="28"/>
+      <c r="B7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="G7" s="27"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2"/>
@@ -3681,10 +4114,10 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="H9" s="12"/>
+      <c r="H9" s="25"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="H10" s="12"/>
+      <c r="H10" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3693,26 +4126,26 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G1 G8:G1048576">
-    <cfRule type="cellIs" dxfId="49" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="5" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="43" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="3" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H10">
-    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3739,148 +4172,148 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="11.875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="23" customWidth="1"/>
-    <col min="3" max="4" width="16.375" style="20" customWidth="1"/>
-    <col min="5" max="5" width="32.625" style="20" customWidth="1"/>
-    <col min="6" max="6" width="61.875" style="20" customWidth="1"/>
-    <col min="7" max="7" width="8.125" style="20" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="20"/>
+    <col min="1" max="1" width="11.875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.875" style="19" customWidth="1"/>
+    <col min="3" max="4" width="16.375" style="16" customWidth="1"/>
+    <col min="5" max="5" width="32.625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="61.875" style="16" customWidth="1"/>
+    <col min="7" max="7" width="8.125" style="16" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="20" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="66">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="G2" s="27"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:8" ht="66">
-      <c r="A3" s="15"/>
-      <c r="B3" s="26" t="s">
+      <c r="A3" s="28"/>
+      <c r="B3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="27"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:8" ht="66">
-      <c r="A4" s="15"/>
-      <c r="B4" s="26" t="s">
+      <c r="A4" s="28"/>
+      <c r="B4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="G4" s="27"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:8" ht="66">
-      <c r="A5" s="15"/>
-      <c r="B5" s="26" t="s">
+      <c r="A5" s="28"/>
+      <c r="B5" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="G5" s="27"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:8" ht="66">
-      <c r="A6" s="15"/>
-      <c r="B6" s="26" t="s">
+      <c r="A6" s="28"/>
+      <c r="B6" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="G6" s="27"/>
+      <c r="G6" s="23"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="21"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="H8" s="12"/>
+      <c r="H8" s="25"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="H9" s="12"/>
+      <c r="H9" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3889,26 +4322,26 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="39" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="7" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="8" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H9">
-    <cfRule type="cellIs" dxfId="37" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="3" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3968,105 +4401,105 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="132">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="28" t="s">
         <v>141</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="28" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="23" t="s">
         <v>142</v>
       </c>
       <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="115.5">
-      <c r="A3" s="15"/>
+      <c r="A3" s="28"/>
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="28"/>
       <c r="D3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="27" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="23" t="s">
         <v>150</v>
       </c>
       <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" ht="115.5">
-      <c r="A4" s="15"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="28" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="23" t="s">
         <v>144</v>
       </c>
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" ht="115.5">
-      <c r="A5" s="15"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="27" t="s">
+      <c r="E5" s="28"/>
+      <c r="F5" s="23" t="s">
         <v>149</v>
       </c>
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" ht="115.5">
-      <c r="A6" s="15"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="28" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="23" t="s">
         <v>147</v>
       </c>
       <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:7" ht="115.5">
-      <c r="A7" s="15"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="27" t="s">
+      <c r="E7" s="28"/>
+      <c r="F7" s="23" t="s">
         <v>148</v>
       </c>
       <c r="G7" s="10"/>
@@ -4083,10 +4516,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4112,269 +4545,269 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="11.875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="23" customWidth="1"/>
-    <col min="3" max="4" width="16.375" style="20" customWidth="1"/>
-    <col min="5" max="5" width="32.625" style="20" customWidth="1"/>
-    <col min="6" max="6" width="61.875" style="20" customWidth="1"/>
-    <col min="7" max="7" width="8.125" style="20" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="20"/>
+    <col min="1" max="1" width="11.875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.875" style="19" customWidth="1"/>
+    <col min="3" max="4" width="16.375" style="16" customWidth="1"/>
+    <col min="5" max="5" width="32.625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="61.875" style="16" customWidth="1"/>
+    <col min="7" max="7" width="8.125" style="16" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="20" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="49.5">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="G2" s="27"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:8" ht="66">
-      <c r="A3" s="15"/>
-      <c r="B3" s="26" t="s">
+      <c r="A3" s="28"/>
+      <c r="B3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="G3" s="27"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:8" ht="66">
-      <c r="A4" s="15"/>
-      <c r="B4" s="26" t="s">
+      <c r="A4" s="28"/>
+      <c r="B4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="23" t="s">
         <v>193</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="G4" s="27"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:8" ht="49.5">
-      <c r="A5" s="15"/>
-      <c r="B5" s="26" t="s">
+      <c r="A5" s="28"/>
+      <c r="B5" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="G5" s="27"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:8" ht="49.5">
-      <c r="A6" s="15"/>
-      <c r="B6" s="26" t="s">
+      <c r="A6" s="28"/>
+      <c r="B6" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="G6" s="27"/>
+      <c r="G6" s="23"/>
     </row>
     <row r="7" spans="1:8" ht="49.5">
-      <c r="A7" s="15"/>
-      <c r="B7" s="26" t="s">
+      <c r="A7" s="28"/>
+      <c r="B7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="23" t="s">
         <v>200</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="G7" s="27"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:8" ht="115.5">
-      <c r="A8" s="15"/>
-      <c r="B8" s="26" t="s">
+      <c r="A8" s="28"/>
+      <c r="B8" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="G8" s="27"/>
-      <c r="H8" s="12"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="25"/>
     </row>
     <row r="9" spans="1:8" ht="66">
-      <c r="A9" s="15"/>
-      <c r="B9" s="26" t="s">
+      <c r="A9" s="28"/>
+      <c r="B9" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="12"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="25"/>
     </row>
     <row r="10" spans="1:8" ht="82.5">
-      <c r="A10" s="15"/>
-      <c r="B10" s="26" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="23" t="s">
         <v>206</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="G10" s="27"/>
+      <c r="G10" s="23"/>
     </row>
     <row r="11" spans="1:8" ht="66">
-      <c r="A11" s="15"/>
-      <c r="B11" s="26" t="s">
+      <c r="A11" s="28"/>
+      <c r="B11" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="G11" s="27"/>
+      <c r="G11" s="23"/>
     </row>
     <row r="12" spans="1:8" ht="66">
-      <c r="A12" s="15"/>
-      <c r="B12" s="26" t="s">
+      <c r="A12" s="28"/>
+      <c r="B12" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="G12" s="27"/>
+      <c r="G12" s="23"/>
     </row>
     <row r="13" spans="1:8" ht="49.5">
-      <c r="A13" s="15"/>
-      <c r="B13" s="26" t="s">
+      <c r="A13" s="28"/>
+      <c r="B13" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="G13" s="27"/>
+      <c r="G13" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4383,114 +4816,114 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="27" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="28" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H9">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="25" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="26" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="23" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="24" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="21" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="22" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="19" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="20" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="17" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="18" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="15" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="16" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="13" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="14" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="11" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="12" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="9" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="10" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="7" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="8" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>